<commit_message>
Update to power plant capacities script as well as new typical units
</commit_message>
<xml_diff>
--- a/GetCapacities/typical_units_chp_matija.xlsx
+++ b/GetCapacities/typical_units_chp_matija.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\dox\DispaSET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\DispaSET---Side-Tools\GetCapacities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A969F28-5883-4349-A6F9-CC9690709BEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6619488-65D8-4D16-BEFC-8F92ECC9A544}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,12 +373,65 @@
         </r>
       </text>
     </comment>
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{9CC32288-7BCB-4DB1-B3BF-109782818834}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Information from the trent 60 datasheet
+https://www.energy.siemens.com/hq/pool/hq/power-generation/gas-turbines/Trent-60/gas-turbine-industrial-trent-60-brochure-en.pdf</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{39D6B2E4-41C1-4894-ABED-66D2A660C195}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Cold start to full power in under 10 minutes according to the datasheet	</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K18" authorId="0" shapeId="0" xr:uid="{AA252D43-6BD6-43B5-A732-2FD2A8E18C1A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Cold start to full power in under 10 minutes according to the datasheet	</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q18" authorId="0" shapeId="0" xr:uid="{93238312-DECD-4EDE-AFC2-7ADDDB0EFEA6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Cold start to full power in under 10 minutes according to the datasheet	</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
   <si>
     <t>PowerCapacity</t>
   </si>
@@ -582,6 +635,9 @@
   </si>
   <si>
     <t>PEA</t>
+  </si>
+  <si>
+    <t>HR_STUR_OTH</t>
   </si>
 </sst>
 </file>
@@ -660,7 +716,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -709,7 +765,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -758,7 +814,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -807,7 +863,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -856,7 +912,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -905,7 +961,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -954,7 +1010,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1003,7 +1059,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1052,7 +1108,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1101,7 +1157,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1150,7 +1206,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1199,7 +1255,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1248,7 +1304,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1297,7 +1353,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1346,7 +1402,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1395,7 +1451,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1444,7 +1500,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1493,7 +1549,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1542,7 +1598,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1591,7 +1647,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1640,7 +1696,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1689,7 +1745,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1738,7 +1794,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1787,7 +1843,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1836,7 +1892,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1885,7 +1941,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1934,7 +1990,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1983,7 +2039,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2032,7 +2088,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2081,7 +2137,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2130,7 +2186,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2179,7 +2235,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2228,7 +2284,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2277,7 +2333,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2326,7 +2382,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2375,7 +2431,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2424,7 +2480,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2473,7 +2529,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2522,7 +2578,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2571,7 +2627,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2620,7 +2676,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2669,7 +2725,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2718,7 +2774,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2767,7 +2823,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2816,7 +2872,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2865,7 +2921,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2914,7 +2970,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2963,7 +3019,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3012,7 +3068,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3061,7 +3117,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3110,7 +3166,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3159,7 +3215,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3208,7 +3264,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3257,7 +3313,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3306,7 +3362,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3355,7 +3411,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3404,7 +3460,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3743,10 +3799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4905,71 +4961,93 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>150</v>
-      </c>
-      <c r="E18" t="s">
+    <row r="18" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>70</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18">
-        <v>0.3</v>
-      </c>
-      <c r="H18">
-        <v>4</v>
-      </c>
-      <c r="I18">
-        <v>4</v>
-      </c>
-      <c r="J18">
-        <v>0.02</v>
-      </c>
-      <c r="K18">
-        <v>0.02</v>
-      </c>
-      <c r="L18">
-        <v>65</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0.5</v>
-      </c>
-      <c r="P18">
-        <v>0.3</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
+      <c r="F18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <f>10/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K18" s="1">
+        <f>10/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="P18" s="1">
+        <f>G18</f>
+        <v>0.33</v>
+      </c>
+      <c r="Q18" s="1">
+        <f>10/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0.79963636400000004</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="U18" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
         <v>50</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J19">
         <v>0.02</v>
@@ -4978,7 +5056,7 @@
         <v>0.02</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -4987,10 +5065,10 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P19">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -5004,13 +5082,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -5019,12 +5097,10 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <f>1/15</f>
-        <v>6.6666666666666666E-2</v>
+        <v>0.02</v>
       </c>
       <c r="K20">
-        <f>1/15</f>
-        <v>6.6666666666666666E-2</v>
+        <v>0.02</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -5046,18 +5122,6 @@
       </c>
       <c r="R20">
         <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
-      </c>
-      <c r="Y20">
-        <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -5065,7 +5129,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
         <v>52</v>
@@ -5118,6 +5182,67 @@
         <v>0</v>
       </c>
       <c r="Y21">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22">
+        <v>0.8</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K22">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
         <v>0.8</v>
       </c>
     </row>

</xml_diff>